<commit_message>
Update GT Workbook by seperating guidelines to assets, create GT  guidelines
</commit_message>
<xml_diff>
--- a/src/module/core/asset/workbook/gtguidelines.xlsx
+++ b/src/module/core/asset/workbook/gtguidelines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Máy tính\New folder\GA-Webapp\src\module\core\asset\workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8C6FCE-2871-430D-97C9-E909AD0719AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0430FB96-B8D4-4B5F-98BC-E3316295BBCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C3A19911-6652-43AB-8F06-65BCE44CA46E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Problem name</t>
   </si>
@@ -57,18 +57,12 @@
     <t>Xác định số người chơi đặc biệt (tạm thời để là 0)</t>
   </si>
   <si>
-    <t>Số người chơi bình thường</t>
-  </si>
-  <si>
     <t>Sheet thứ 2: Normal players</t>
   </si>
   <si>
     <t>Player name (nếu bỏ trống thì sẽ được coi là Player n)</t>
   </si>
   <si>
-    <t>Hàm tính payoff của chiến lược chung</t>
-  </si>
-  <si>
     <t>thuộc tính 2</t>
   </si>
   <si>
@@ -82,21 +76,10 @@
   </si>
   <si>
     <t>Sheet thứ 3: Conflicts matrix</t>
-  </si>
-  <si>
-    <t>player 1, strategy 1, player 2, strategy 2</t>
   </si>
   <si>
     <t>Số thuộc tính của chiến lược mà người chơi đặc 
 biệt chịu ảnh hưởng</t>
-  </si>
-  <si>
-    <t>Số thuộc tính của chiến lược mà người chơi bình 
-thường chịu ảnh hưởng</t>
-  </si>
-  <si>
-    <t>Hàm tính điểm hài lòng của người chơi với chiến 
-lược đưa ra, nếu bỏ không thì sẽ tính theo default</t>
   </si>
   <si>
     <t>Hàm tính điểm payoff của chiến lược người chơi 
@@ -118,23 +101,68 @@
     <t>Strategy Name 1 (Tên chiến lược đưa ra)</t>
   </si>
   <si>
-    <t>thuộc tính 1, thuộc tính 2, thuộc tính n</t>
-  </si>
-  <si>
-    <t>Số chiến lược của người chơi, hàm payoff của người chơi đó (nếu có)</t>
-  </si>
-  <si>
     <t>HƯỚNG DẪN CÁCH ĐIỀN FORM GAME THEORY</t>
   </si>
   <si>
     <t>Sheet 1: Problem name</t>
+  </si>
+  <si>
+    <t>thuộc tính 1</t>
+  </si>
+  <si>
+    <t>Số chiến lược của người chơi</t>
+  </si>
+  <si>
+    <t>FINDING NEMO GAME</t>
+  </si>
+  <si>
+    <t>Số người chơi bình thường, min là 2 max là 
+1000 (current)</t>
+  </si>
+  <si>
+    <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>Hàm tính điểm hài lòng của người chơi với chiến 
+lược đưa ra, nếu bỏ không thì sẽ điền "DEFAULT"
+(check manual để tìm hiểu các phép toán được hỗ trợ)</t>
+  </si>
+  <si>
+    <t>p1 + p2 + p3 - p4</t>
+  </si>
+  <si>
+    <t>Player 1</t>
+  </si>
+  <si>
+    <t>Vườn không nhà trống</t>
+  </si>
+  <si>
+    <t>Kháng chiến toàn dân</t>
+  </si>
+  <si>
+    <t>Hàm payoff của người chơi đó (nếu có, không thì 
+default, được phép bỏ trống)</t>
+  </si>
+  <si>
+    <t>Player 1, vườn không nhà trống, player 2, biển người vô tận</t>
+  </si>
+  <si>
+    <t>player a, strategy x (of a), player b, strategy z (of b)</t>
+  </si>
+  <si>
+    <t>VÍ DỤ</t>
+  </si>
+  <si>
+    <t>Số thuộc tính của chiến lược mà người chơi bình 
+thường chịu ảnh hưởng ( &gt;= 1) (số lượng thuộc tính 
+của các chiến lược luôn phải bằng nhau)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,30 +172,43 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0099CC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -183,12 +224,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF5050"/>
+        <fgColor rgb="FFCCECFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -301,43 +354,223 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,6 +579,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCCECFF"/>
       <color rgb="FFCCCCFF"/>
       <color rgb="FFFF5050"/>
       <color rgb="FF99CCFF"/>
@@ -662,240 +896,349 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DE00F74-2956-4B3B-ADAA-6B69A9B72986}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="2" width="55.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.33203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="3.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18"/>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="43"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="46"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="34"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="39">
+        <v>0</v>
+      </c>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="34"/>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="39">
+        <v>0</v>
+      </c>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="34"/>
+    </row>
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="39">
+        <v>10</v>
+      </c>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="34"/>
+    </row>
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="39">
+        <v>4</v>
+      </c>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="34"/>
+    </row>
+    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="34"/>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="34"/>
+    </row>
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="34"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
-    </row>
-    <row r="8" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-    </row>
-    <row r="9" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
-    </row>
-    <row r="10" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="49"/>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
+      <c r="B12" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="19"/>
       <c r="E12" s="20"/>
       <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="G12" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="30">
+        <v>2</v>
+      </c>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="32"/>
+    </row>
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="E13" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="F13" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="G13" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="33">
+        <v>10</v>
+      </c>
+      <c r="I13" s="29">
+        <v>10</v>
+      </c>
+      <c r="J13" s="29">
+        <v>10</v>
+      </c>
+      <c r="K13" s="34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="35">
+        <v>20</v>
+      </c>
+      <c r="I14" s="36">
+        <v>20</v>
+      </c>
+      <c r="J14" s="36">
+        <v>20</v>
+      </c>
+      <c r="K14" s="37">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="21"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="10"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="49"/>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>